<commit_message>
added possibility to close sprints
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,7 +1728,7 @@
         <v>26</v>
       </c>
       <c r="D78" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>28</v>
       </c>
       <c r="D84" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
         <v>28</v>
       </c>
       <c r="D85" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final version, working on Vadim's local Jira
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1">
         <v>11</v>
@@ -1092,7 +1092,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
         <v>11</v>
@@ -1106,7 +1106,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1">
         <v>11</v>
@@ -1134,7 +1134,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C36" s="1">
         <v>12</v>
@@ -1162,7 +1162,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
         <v>13</v>
@@ -1190,7 +1190,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C40" s="1">
         <v>13</v>
@@ -1204,7 +1204,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C41" s="1">
         <v>14</v>
@@ -1218,7 +1218,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1">
         <v>14</v>
@@ -1232,7 +1232,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1">
         <v>14</v>
@@ -1246,7 +1246,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1">
         <v>15</v>
@@ -1274,7 +1274,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1">
         <v>15</v>
@@ -1302,7 +1302,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1">
         <v>16</v>
@@ -1330,7 +1330,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C50" s="1">
         <v>17</v>
@@ -1344,7 +1344,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C51" s="1">
         <v>17</v>
@@ -1358,7 +1358,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C52" s="1">
         <v>17</v>
@@ -1386,7 +1386,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C54" s="1">
         <v>18</v>
@@ -1414,7 +1414,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C56" s="1">
         <v>19</v>
@@ -1428,7 +1428,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C57" s="1">
         <v>19</v>
@@ -1442,7 +1442,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1">
         <v>19</v>
@@ -1470,7 +1470,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C60" s="1">
         <v>20</v>
@@ -1484,7 +1484,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C61" s="1">
         <v>20</v>
@@ -1498,7 +1498,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C62" s="1">
         <v>21</v>
@@ -1512,7 +1512,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C63" s="1">
         <v>21</v>
@@ -1526,7 +1526,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C64" s="1">
         <v>21</v>
@@ -1540,7 +1540,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C65" s="1">
         <v>22</v>
@@ -1568,7 +1568,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C67" s="1">
         <v>22</v>
@@ -1582,7 +1582,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C68" s="1">
         <v>23</v>
@@ -1610,7 +1610,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C70" s="1">
         <v>23</v>
@@ -1624,7 +1624,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C71" s="1">
         <v>24</v>
@@ -1638,7 +1638,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C72" s="1">
         <v>24</v>
@@ -1666,7 +1666,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C74" s="1">
         <v>25</v>
@@ -1694,7 +1694,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C76" s="1">
         <v>25</v>
@@ -1708,7 +1708,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C77" s="1">
         <v>26</v>
@@ -1722,7 +1722,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C78" s="1">
         <v>26</v>
@@ -1736,7 +1736,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C79" s="1">
         <v>26</v>
@@ -1764,7 +1764,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C81" s="1">
         <v>27</v>
@@ -1778,7 +1778,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C82" s="1">
         <v>27</v>
@@ -1792,7 +1792,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C83" s="1">
         <v>28</v>
@@ -1820,7 +1820,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C85" s="1">
         <v>28</v>
@@ -1834,7 +1834,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C86" s="1">
         <v>29</v>
@@ -1848,7 +1848,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C87" s="1">
         <v>29</v>
@@ -1862,7 +1862,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C88" s="1">
         <v>29</v>
@@ -1876,7 +1876,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C89" s="1">
         <v>30</v>
@@ -1904,7 +1904,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C91" s="1">
         <v>30</v>

</xml_diff>